<commit_message>
Piege MAJ + coordonnées de la team
</commit_message>
<xml_diff>
--- a/Piege.xlsx
+++ b/Piege.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Piege</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Racine au sol</t>
   </si>
   <si>
-    <t>Déstruction des racine</t>
-  </si>
-  <si>
-    <t>Feulle grimpante</t>
-  </si>
-  <si>
     <t>Découper</t>
   </si>
   <si>
@@ -51,9 +45,6 @@
     <t>Singe qui lance des noix de coco</t>
   </si>
   <si>
-    <t>Placer un boulier ou autre pour faire "Paraplui"</t>
-  </si>
-  <si>
     <t>Boulet qui tombe d'une montagne</t>
   </si>
   <si>
@@ -75,7 +66,52 @@
     <t xml:space="preserve">Feu </t>
   </si>
   <si>
-    <t>Clicker pour résuire la vie du feu</t>
+    <t>Destruction des racines</t>
+  </si>
+  <si>
+    <t>Placer un bouclier ou autre pour faire "Paraplui"</t>
+  </si>
+  <si>
+    <t>Feuille grimpante</t>
+  </si>
+  <si>
+    <t>Cliquer pour réduire la vie du feu</t>
+  </si>
+  <si>
+    <t>Attaque distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attaque à bout portant </t>
+  </si>
+  <si>
+    <t>Cliquer pour enlever</t>
+  </si>
+  <si>
+    <t>Attaque venant du ciel (pluie, bulles, cercles de fumée, animaux, objets, nourriture...)</t>
+  </si>
+  <si>
+    <t>Qui foncent en ligne droite ou zigzag sur le personnage ("")</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>Objets roulant : Boule de neige (montagne), tronc d'arbre (foret)</t>
+  </si>
+  <si>
+    <t>Cliquer pour le dévier les objets</t>
+  </si>
+  <si>
+    <t>Sol modifié  : Boue -&gt; pieds qui s'enfoncent (foret), marshmallow nuage (sol collant caramel), glisse (montagne)</t>
+  </si>
+  <si>
+    <t>Cliquer pour détruire/tuer</t>
+  </si>
+  <si>
+    <t>Vide/trou</t>
+  </si>
+  <si>
+    <t>Mettre une planche</t>
   </si>
 </sst>
 </file>
@@ -414,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B12"/>
+  <dimension ref="A2:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="92.88671875" customWidth="1"/>
     <col min="2" max="2" width="58.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -447,63 +483,116 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>